<commit_message>
chore: Update binary files for .DS_Store and Chesterton_SQM-2.xlsx
</commit_message>
<xml_diff>
--- a/Seal-Reparation/Chesterton_SQM-2.xlsx
+++ b/Seal-Reparation/Chesterton_SQM-2.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10608"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10817"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sebastianconcha/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sebastianconcha/Developer/Chesterton2025/Seal-Reparation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83DAADF8-2581-FA40-BC96-1C0805C4E4BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDD860FB-CEB3-254B-A062-E2B6B3E83057}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -6761,7 +6761,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5915" uniqueCount="1289">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6416" uniqueCount="1465">
   <si>
     <t>id</t>
   </si>
@@ -10655,6 +10655,534 @@
   </si>
   <si>
     <t>Sello mecánico cambiado con éxito</t>
+  </si>
+  <si>
+    <t>SC4946</t>
+  </si>
+  <si>
+    <t>8/27/2025 16:48:21</t>
+  </si>
+  <si>
+    <t>SC4947</t>
+  </si>
+  <si>
+    <t>8/28/2025 13:50:27</t>
+  </si>
+  <si>
+    <t>SC4948</t>
+  </si>
+  <si>
+    <t>8/28/2025 14:07:24</t>
+  </si>
+  <si>
+    <t>SC4949</t>
+  </si>
+  <si>
+    <t>8/28/2025 15:18:27</t>
+  </si>
+  <si>
+    <t>SC4950</t>
+  </si>
+  <si>
+    <t>8/28/2025 16:38:13</t>
+  </si>
+  <si>
+    <t>SC4951</t>
+  </si>
+  <si>
+    <t>SC4952</t>
+  </si>
+  <si>
+    <t>SC4953</t>
+  </si>
+  <si>
+    <t>SC4954</t>
+  </si>
+  <si>
+    <t>SC4955</t>
+  </si>
+  <si>
+    <t>SC4957</t>
+  </si>
+  <si>
+    <t>SC4958</t>
+  </si>
+  <si>
+    <t>SC4956</t>
+  </si>
+  <si>
+    <t>Sc5004</t>
+  </si>
+  <si>
+    <t>SC5005</t>
+  </si>
+  <si>
+    <t>SC5006</t>
+  </si>
+  <si>
+    <t>SC5007</t>
+  </si>
+  <si>
+    <t>SC5008</t>
+  </si>
+  <si>
+    <t>SC5009</t>
+  </si>
+  <si>
+    <t>SC5010</t>
+  </si>
+  <si>
+    <t>SC5011</t>
+  </si>
+  <si>
+    <t>SC5012</t>
+  </si>
+  <si>
+    <t>SC5013</t>
+  </si>
+  <si>
+    <t>SC5014</t>
+  </si>
+  <si>
+    <t>SC5017</t>
+  </si>
+  <si>
+    <t>SC5016</t>
+  </si>
+  <si>
+    <t>SC5018</t>
+  </si>
+  <si>
+    <t>SC5015</t>
+  </si>
+  <si>
+    <t>SC5020</t>
+  </si>
+  <si>
+    <t>SC5019</t>
+  </si>
+  <si>
+    <t>SC5021</t>
+  </si>
+  <si>
+    <t>SC5022</t>
+  </si>
+  <si>
+    <t>SC5023</t>
+  </si>
+  <si>
+    <t>SC5024</t>
+  </si>
+  <si>
+    <t>SC5025</t>
+  </si>
+  <si>
+    <t>SC5026</t>
+  </si>
+  <si>
+    <t>SC5027</t>
+  </si>
+  <si>
+    <t>185512CL - S10/OS 2.500 SA TC/SSC SS316 FEPM Kit completo Grasa</t>
+  </si>
+  <si>
+    <t>SC5028</t>
+  </si>
+  <si>
+    <t>SC5029</t>
+  </si>
+  <si>
+    <t>https://chesterton.operations.dynamics.com/?cmp=019&amp;mi=ProdTableListPage</t>
+  </si>
+  <si>
+    <t>SC5040</t>
+  </si>
+  <si>
+    <t>9/26/2025 16:12:02</t>
+  </si>
+  <si>
+    <t>SC5036</t>
+  </si>
+  <si>
+    <t>9/26/2025 16:19:34</t>
+  </si>
+  <si>
+    <t>SC5033</t>
+  </si>
+  <si>
+    <t>9/26/2025 16:27:10</t>
+  </si>
+  <si>
+    <t>SC5032</t>
+  </si>
+  <si>
+    <t>9/26/2025 16:33:58</t>
+  </si>
+  <si>
+    <t>SC5030</t>
+  </si>
+  <si>
+    <t>9/26/2025 16:40:50</t>
+  </si>
+  <si>
+    <t>SC4851</t>
+  </si>
+  <si>
+    <t>9/26/2025 16:46:43</t>
+  </si>
+  <si>
+    <t>SC5042</t>
+  </si>
+  <si>
+    <t>9/26/2025 16:53:26</t>
+  </si>
+  <si>
+    <t>SC5039</t>
+  </si>
+  <si>
+    <t>9/26/2025 17:03:35</t>
+  </si>
+  <si>
+    <t>SC5051</t>
+  </si>
+  <si>
+    <t>9/26/2025 17:27:50</t>
+  </si>
+  <si>
+    <t>SC4021</t>
+  </si>
+  <si>
+    <t>9/26/2025 17:34:11</t>
+  </si>
+  <si>
+    <t>SC4430</t>
+  </si>
+  <si>
+    <t>9/26/2025 17:38:56</t>
+  </si>
+  <si>
+    <t>SC5054</t>
+  </si>
+  <si>
+    <t>9/26/2025 17:43:09</t>
+  </si>
+  <si>
+    <t>SC5044</t>
+  </si>
+  <si>
+    <t>9/26/2025 17:54:21</t>
+  </si>
+  <si>
+    <t>9/26/2025 17:57:48</t>
+  </si>
+  <si>
+    <t>SC5041</t>
+  </si>
+  <si>
+    <t>9/30/2025 12:01:41</t>
+  </si>
+  <si>
+    <t>SC3981</t>
+  </si>
+  <si>
+    <t>9/30/2025 12:07:09</t>
+  </si>
+  <si>
+    <t>SC5035</t>
+  </si>
+  <si>
+    <t>9/30/2025 12:16:20</t>
+  </si>
+  <si>
+    <t>SC5037</t>
+  </si>
+  <si>
+    <t>9/30/2025 13:21:42</t>
+  </si>
+  <si>
+    <t>SC5034</t>
+  </si>
+  <si>
+    <t>9/30/2025 13:25:58</t>
+  </si>
+  <si>
+    <t>SC5043</t>
+  </si>
+  <si>
+    <t>9/30/2025 13:30:46</t>
+  </si>
+  <si>
+    <t>SC5038</t>
+  </si>
+  <si>
+    <t>9/30/2025 13:37:20</t>
+  </si>
+  <si>
+    <t>SC5031</t>
+  </si>
+  <si>
+    <t>9/30/2025 14:39:15</t>
+  </si>
+  <si>
+    <t>SC5046</t>
+  </si>
+  <si>
+    <t>9/30/2025 14:46:48</t>
+  </si>
+  <si>
+    <t>SC5058</t>
+  </si>
+  <si>
+    <t>9/30/2025 14:50:58</t>
+  </si>
+  <si>
+    <t>SC5048</t>
+  </si>
+  <si>
+    <t>9/30/2025 15:00:33</t>
+  </si>
+  <si>
+    <t>SC5045</t>
+  </si>
+  <si>
+    <t>9/30/2025 15:03:23</t>
+  </si>
+  <si>
+    <t>SC5050</t>
+  </si>
+  <si>
+    <t>9/30/2025 15:08:45</t>
+  </si>
+  <si>
+    <t>SC5057</t>
+  </si>
+  <si>
+    <t>9/30/2025 15:12:38</t>
+  </si>
+  <si>
+    <t>SC5052</t>
+  </si>
+  <si>
+    <t>9/30/2025 15:53:36</t>
+  </si>
+  <si>
+    <t>SC5047</t>
+  </si>
+  <si>
+    <t>9/30/2025 15:56:52</t>
+  </si>
+  <si>
+    <t>SC5056</t>
+  </si>
+  <si>
+    <t>9/30/2025 16:00:39</t>
+  </si>
+  <si>
+    <t>SC5055</t>
+  </si>
+  <si>
+    <t>9/30/2025 16:05:58</t>
+  </si>
+  <si>
+    <t>SC5059</t>
+  </si>
+  <si>
+    <t>9/30/2025 16:11:13</t>
+  </si>
+  <si>
+    <t>SC5049</t>
+  </si>
+  <si>
+    <t>9/30/2025 16:14:31</t>
+  </si>
+  <si>
+    <t>10/30/2025 10:51:13</t>
+  </si>
+  <si>
+    <t>SC5077</t>
+  </si>
+  <si>
+    <t>10/30/2025 11:00:22</t>
+  </si>
+  <si>
+    <t>SC5076</t>
+  </si>
+  <si>
+    <t>10/30/2025 11:09:26</t>
+  </si>
+  <si>
+    <t>SC5078</t>
+  </si>
+  <si>
+    <t>Trabajo en seco prolongado</t>
+  </si>
+  <si>
+    <t>10/30/2025 11:19:06</t>
+  </si>
+  <si>
+    <t>SC5084</t>
+  </si>
+  <si>
+    <t>10/30/2025 11:53:22</t>
+  </si>
+  <si>
+    <t>10/30/2025 12:01:43</t>
+  </si>
+  <si>
+    <t>SC5079</t>
+  </si>
+  <si>
+    <t>10/30/2025 12:06:32</t>
+  </si>
+  <si>
+    <t>SC5082</t>
+  </si>
+  <si>
+    <t>10/30/2025 12:09:51</t>
+  </si>
+  <si>
+    <t>10/30/2025 12:14:00</t>
+  </si>
+  <si>
+    <t>SC5083</t>
+  </si>
+  <si>
+    <t>10/30/2025 12:24:05</t>
+  </si>
+  <si>
+    <t>SC5080</t>
+  </si>
+  <si>
+    <t>10/30/2025 12:40:08</t>
+  </si>
+  <si>
+    <t>SC5081</t>
+  </si>
+  <si>
+    <t>10/30/2025 12:46:31</t>
+  </si>
+  <si>
+    <t>SC3983</t>
+  </si>
+  <si>
+    <t>10/30/2025 12:51:24</t>
+  </si>
+  <si>
+    <t>SC5069</t>
+  </si>
+  <si>
+    <t>10/30/2025 12:54:37</t>
+  </si>
+  <si>
+    <t>SC5072</t>
+  </si>
+  <si>
+    <t>10/30/2025 13:00:34</t>
+  </si>
+  <si>
+    <t>SC5061</t>
+  </si>
+  <si>
+    <t>10/30/2025 13:06:37</t>
+  </si>
+  <si>
+    <t>10/30/2025 13:13:54</t>
+  </si>
+  <si>
+    <t>SC5066</t>
+  </si>
+  <si>
+    <t>10/30/2025 13:18:39</t>
+  </si>
+  <si>
+    <t>SC5070</t>
+  </si>
+  <si>
+    <t>10/30/2025 13:23:32</t>
+  </si>
+  <si>
+    <t>SC5065</t>
+  </si>
+  <si>
+    <t>10/30/2025 13:27:59</t>
+  </si>
+  <si>
+    <t>SC5073</t>
+  </si>
+  <si>
+    <t>10/30/2025 13:31:30</t>
+  </si>
+  <si>
+    <t>10/30/2025 13:36:55</t>
+  </si>
+  <si>
+    <t>SC5064</t>
+  </si>
+  <si>
+    <t>10/30/2025 15:18:23</t>
+  </si>
+  <si>
+    <t>SC5062</t>
+  </si>
+  <si>
+    <t>10/30/2025 15:31:33</t>
+  </si>
+  <si>
+    <t>SC5060</t>
+  </si>
+  <si>
+    <t>10/30/2025 15:38:39</t>
+  </si>
+  <si>
+    <t>SC5074</t>
+  </si>
+  <si>
+    <t>10/30/2025 16:00:32</t>
+  </si>
+  <si>
+    <t>SC5085</t>
+  </si>
+  <si>
+    <t>10/30/2025 16:10:02</t>
+  </si>
+  <si>
+    <t>SC5068</t>
+  </si>
+  <si>
+    <t>10/30/2025 17:19:45</t>
+  </si>
+  <si>
+    <t>SC5075</t>
+  </si>
+  <si>
+    <t>10/30/2025 17:25:37</t>
+  </si>
+  <si>
+    <t>SC5071</t>
+  </si>
+  <si>
+    <t>10/30/2025 17:29:56</t>
+  </si>
+  <si>
+    <t>10/30/2025 17:39:19</t>
+  </si>
+  <si>
+    <t>10/30/2025 17:46:55</t>
+  </si>
+  <si>
+    <t>SC5063</t>
+  </si>
+  <si>
+    <t>866005CL - S10 1.375 SA TC/SSC Alloy20 FEPM KIT completo Grasa</t>
+  </si>
+  <si>
+    <t>10/30/2025 17:52:28</t>
+  </si>
+  <si>
+    <t>SC3799</t>
+  </si>
+  <si>
+    <t>10/30/2025 17:58:35</t>
   </si>
 </sst>
 </file>
@@ -10664,7 +11192,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="m/d/yyyy\ h:mm:ss"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -10687,6 +11215,19 @@
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF434343"/>
+      <name val="Roboto"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="10"/>
       <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -10901,10 +11442,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -10962,8 +11504,12 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="22" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="3">
@@ -11011,7 +11557,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Recepcion" displayName="Recepcion" ref="A1:F157">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Recepcion" displayName="Recepcion" ref="A1:F264">
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="SC"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Modelo"/>
@@ -11354,10 +11900,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:F157"/>
+  <dimension ref="A1:F264"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I29" sqref="I29"/>
+      <selection activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -15288,15 +15834,2158 @@
         <v>5</v>
       </c>
     </row>
+    <row r="158" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A158" s="21" t="s">
+        <v>1289</v>
+      </c>
+      <c r="B158" s="21" t="s">
+        <v>453</v>
+      </c>
+      <c r="C158" s="21" t="s">
+        <v>167</v>
+      </c>
+      <c r="D158" s="21" t="s">
+        <v>115</v>
+      </c>
+      <c r="E158" s="21" t="s">
+        <v>1290</v>
+      </c>
+      <c r="F158" s="21">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="159" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A159" s="21" t="s">
+        <v>1291</v>
+      </c>
+      <c r="B159" s="21" t="s">
+        <v>91</v>
+      </c>
+      <c r="C159" s="21" t="s">
+        <v>169</v>
+      </c>
+      <c r="D159" s="21" t="s">
+        <v>115</v>
+      </c>
+      <c r="E159" s="21" t="s">
+        <v>1292</v>
+      </c>
+      <c r="F159" s="21">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="160" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A160" s="21" t="s">
+        <v>1293</v>
+      </c>
+      <c r="B160" s="21" t="s">
+        <v>91</v>
+      </c>
+      <c r="C160" s="21" t="s">
+        <v>90</v>
+      </c>
+      <c r="D160" s="21" t="s">
+        <v>149</v>
+      </c>
+      <c r="E160" s="21" t="s">
+        <v>1294</v>
+      </c>
+      <c r="F160" s="21">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="161" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A161" s="21" t="s">
+        <v>1295</v>
+      </c>
+      <c r="B161" s="21" t="s">
+        <v>91</v>
+      </c>
+      <c r="C161" s="21" t="s">
+        <v>167</v>
+      </c>
+      <c r="D161" s="21" t="s">
+        <v>121</v>
+      </c>
+      <c r="E161" s="21" t="s">
+        <v>1296</v>
+      </c>
+      <c r="F161" s="21">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="162" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A162" s="21" t="s">
+        <v>1297</v>
+      </c>
+      <c r="B162" s="21" t="s">
+        <v>91</v>
+      </c>
+      <c r="C162" s="21" t="s">
+        <v>125</v>
+      </c>
+      <c r="D162" s="21" t="s">
+        <v>121</v>
+      </c>
+      <c r="E162" s="21" t="s">
+        <v>1298</v>
+      </c>
+      <c r="F162" s="21">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="163" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A163" s="21" t="s">
+        <v>1299</v>
+      </c>
+      <c r="B163" s="21" t="s">
+        <v>91</v>
+      </c>
+      <c r="C163" s="21" t="s">
+        <v>167</v>
+      </c>
+      <c r="D163" s="21" t="s">
+        <v>115</v>
+      </c>
+      <c r="E163" s="22">
+        <v>45697.576249999998</v>
+      </c>
+      <c r="F163" s="21">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="164" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A164" s="21" t="s">
+        <v>1300</v>
+      </c>
+      <c r="B164" s="21" t="s">
+        <v>91</v>
+      </c>
+      <c r="C164" s="21" t="s">
+        <v>167</v>
+      </c>
+      <c r="D164" s="21" t="s">
+        <v>121</v>
+      </c>
+      <c r="E164" s="22">
+        <v>45697.598495370374</v>
+      </c>
+      <c r="F164" s="21">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="165" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A165" s="21" t="s">
+        <v>1301</v>
+      </c>
+      <c r="B165" s="21" t="s">
+        <v>86</v>
+      </c>
+      <c r="C165" s="21" t="s">
+        <v>125</v>
+      </c>
+      <c r="D165" s="21" t="s">
+        <v>121</v>
+      </c>
+      <c r="E165" s="22">
+        <v>45697.627372685187</v>
+      </c>
+      <c r="F165" s="21">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="166" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A166" s="21" t="s">
+        <v>1302</v>
+      </c>
+      <c r="B166" s="21" t="s">
+        <v>86</v>
+      </c>
+      <c r="C166" s="21" t="s">
+        <v>90</v>
+      </c>
+      <c r="D166" s="21" t="s">
+        <v>121</v>
+      </c>
+      <c r="E166" s="22">
+        <v>45697.631967592592</v>
+      </c>
+      <c r="F166" s="21">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="167" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A167" s="21" t="s">
+        <v>1303</v>
+      </c>
+      <c r="B167" s="21" t="s">
+        <v>86</v>
+      </c>
+      <c r="C167" s="21" t="s">
+        <v>125</v>
+      </c>
+      <c r="D167" s="21" t="s">
+        <v>121</v>
+      </c>
+      <c r="E167" s="22">
+        <v>45697.644178240742</v>
+      </c>
+      <c r="F167" s="21">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="168" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A168" s="21" t="s">
+        <v>1304</v>
+      </c>
+      <c r="B168" s="21" t="s">
+        <v>86</v>
+      </c>
+      <c r="C168" s="21" t="s">
+        <v>125</v>
+      </c>
+      <c r="D168" s="21" t="s">
+        <v>121</v>
+      </c>
+      <c r="E168" s="22">
+        <v>45697.666944444441</v>
+      </c>
+      <c r="F168" s="21">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="169" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A169" s="21" t="s">
+        <v>1305</v>
+      </c>
+      <c r="B169" s="21" t="s">
+        <v>86</v>
+      </c>
+      <c r="C169" s="21" t="s">
+        <v>184</v>
+      </c>
+      <c r="D169" s="21" t="s">
+        <v>121</v>
+      </c>
+      <c r="E169" s="22">
+        <v>45697.675011574072</v>
+      </c>
+      <c r="F169" s="21">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="170" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A170" s="21" t="s">
+        <v>1306</v>
+      </c>
+      <c r="B170" s="21" t="s">
+        <v>91</v>
+      </c>
+      <c r="C170" s="21" t="s">
+        <v>259</v>
+      </c>
+      <c r="D170" s="21" t="s">
+        <v>121</v>
+      </c>
+      <c r="E170" s="22">
+        <v>45697.662986111114</v>
+      </c>
+      <c r="F170" s="21">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="171" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A171" s="21" t="s">
+        <v>1307</v>
+      </c>
+      <c r="B171" s="21" t="s">
+        <v>221</v>
+      </c>
+      <c r="C171" s="21" t="s">
+        <v>169</v>
+      </c>
+      <c r="D171" s="21" t="s">
+        <v>115</v>
+      </c>
+      <c r="E171" s="22">
+        <v>45697.701701388891</v>
+      </c>
+      <c r="F171" s="21">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="172" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A172" s="21" t="s">
+        <v>1308</v>
+      </c>
+      <c r="B172" s="21" t="s">
+        <v>161</v>
+      </c>
+      <c r="C172" s="21" t="s">
+        <v>169</v>
+      </c>
+      <c r="D172" s="21" t="s">
+        <v>115</v>
+      </c>
+      <c r="E172" s="22">
+        <v>45697.703541666669</v>
+      </c>
+      <c r="F172" s="21">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="173" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A173" s="21" t="s">
+        <v>1309</v>
+      </c>
+      <c r="B173" s="21" t="s">
+        <v>100</v>
+      </c>
+      <c r="C173" s="21" t="s">
+        <v>90</v>
+      </c>
+      <c r="D173" s="21" t="s">
+        <v>149</v>
+      </c>
+      <c r="E173" s="22">
+        <v>45697.706597222219</v>
+      </c>
+      <c r="F173" s="21">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="174" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A174" s="21" t="s">
+        <v>1310</v>
+      </c>
+      <c r="B174" s="21" t="s">
+        <v>100</v>
+      </c>
+      <c r="C174" s="21" t="s">
+        <v>125</v>
+      </c>
+      <c r="D174" s="21" t="s">
+        <v>121</v>
+      </c>
+      <c r="E174" s="22">
+        <v>45697.709803240738</v>
+      </c>
+      <c r="F174" s="21">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="175" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A175" s="21" t="s">
+        <v>1311</v>
+      </c>
+      <c r="B175" s="21" t="s">
+        <v>100</v>
+      </c>
+      <c r="C175" s="21" t="s">
+        <v>291</v>
+      </c>
+      <c r="D175" s="21" t="s">
+        <v>115</v>
+      </c>
+      <c r="E175" s="22">
+        <v>45697.730046296296</v>
+      </c>
+      <c r="F175" s="21">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="176" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A176" s="21" t="s">
+        <v>1312</v>
+      </c>
+      <c r="B176" s="21" t="s">
+        <v>100</v>
+      </c>
+      <c r="C176" s="21" t="s">
+        <v>184</v>
+      </c>
+      <c r="D176" s="21" t="s">
+        <v>121</v>
+      </c>
+      <c r="E176" s="22">
+        <v>45697.741597222222</v>
+      </c>
+      <c r="F176" s="21">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="177" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A177" s="21" t="s">
+        <v>1313</v>
+      </c>
+      <c r="B177" s="21" t="s">
+        <v>100</v>
+      </c>
+      <c r="C177" s="21" t="s">
+        <v>212</v>
+      </c>
+      <c r="D177" s="21" t="s">
+        <v>121</v>
+      </c>
+      <c r="E177" s="22">
+        <v>45697.744189814817</v>
+      </c>
+      <c r="F177" s="21">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="178" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A178" s="21" t="s">
+        <v>1314</v>
+      </c>
+      <c r="B178" s="21" t="s">
+        <v>100</v>
+      </c>
+      <c r="C178" s="21" t="s">
+        <v>291</v>
+      </c>
+      <c r="D178" s="21" t="s">
+        <v>149</v>
+      </c>
+      <c r="E178" s="22">
+        <v>45697.753333333334</v>
+      </c>
+      <c r="F178" s="21">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="179" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A179" s="21" t="s">
+        <v>1315</v>
+      </c>
+      <c r="B179" s="21" t="s">
+        <v>100</v>
+      </c>
+      <c r="C179" s="21" t="s">
+        <v>169</v>
+      </c>
+      <c r="D179" s="21" t="s">
+        <v>149</v>
+      </c>
+      <c r="E179" s="22">
+        <v>45697.758229166669</v>
+      </c>
+      <c r="F179" s="21">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="180" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A180" s="21" t="s">
+        <v>1316</v>
+      </c>
+      <c r="B180" s="21" t="s">
+        <v>100</v>
+      </c>
+      <c r="C180" s="21" t="s">
+        <v>291</v>
+      </c>
+      <c r="D180" s="21" t="s">
+        <v>115</v>
+      </c>
+      <c r="E180" s="22">
+        <v>45697.764918981484</v>
+      </c>
+      <c r="F180" s="21">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="181" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A181" s="21" t="s">
+        <v>1317</v>
+      </c>
+      <c r="B181" s="21" t="s">
+        <v>100</v>
+      </c>
+      <c r="C181" s="21" t="s">
+        <v>125</v>
+      </c>
+      <c r="D181" s="21" t="s">
+        <v>121</v>
+      </c>
+      <c r="E181" s="22">
+        <v>45697.787685185183</v>
+      </c>
+      <c r="F181" s="21">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="182" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A182" s="21" t="s">
+        <v>1318</v>
+      </c>
+      <c r="B182" s="21" t="s">
+        <v>100</v>
+      </c>
+      <c r="C182" s="21" t="s">
+        <v>409</v>
+      </c>
+      <c r="D182" s="21" t="s">
+        <v>121</v>
+      </c>
+      <c r="E182" s="22">
+        <v>45697.823240740741</v>
+      </c>
+      <c r="F182" s="21">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="183" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A183" s="21" t="s">
+        <v>1319</v>
+      </c>
+      <c r="B183" s="21" t="s">
+        <v>100</v>
+      </c>
+      <c r="C183" s="21" t="s">
+        <v>153</v>
+      </c>
+      <c r="D183" s="21" t="s">
+        <v>115</v>
+      </c>
+      <c r="E183" s="22">
+        <v>45697.80159722222</v>
+      </c>
+      <c r="F183" s="21">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="184" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A184" s="21" t="s">
+        <v>1320</v>
+      </c>
+      <c r="B184" s="21" t="s">
+        <v>100</v>
+      </c>
+      <c r="C184" s="21" t="s">
+        <v>169</v>
+      </c>
+      <c r="D184" s="21" t="s">
+        <v>121</v>
+      </c>
+      <c r="E184" s="22">
+        <v>45697.814293981479</v>
+      </c>
+      <c r="F184" s="21">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="185" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A185" s="21" t="s">
+        <v>1321</v>
+      </c>
+      <c r="B185" s="21" t="s">
+        <v>100</v>
+      </c>
+      <c r="C185" s="21" t="s">
+        <v>125</v>
+      </c>
+      <c r="D185" s="21" t="s">
+        <v>121</v>
+      </c>
+      <c r="E185" s="22">
+        <v>45697.793194444443</v>
+      </c>
+      <c r="F185" s="21">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="186" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A186" s="21" t="s">
+        <v>1322</v>
+      </c>
+      <c r="B186" s="21" t="s">
+        <v>100</v>
+      </c>
+      <c r="C186" s="21" t="s">
+        <v>167</v>
+      </c>
+      <c r="D186" s="21" t="s">
+        <v>121</v>
+      </c>
+      <c r="E186" s="22">
+        <v>45697.831261574072</v>
+      </c>
+      <c r="F186" s="21">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="187" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A187" s="21" t="s">
+        <v>1323</v>
+      </c>
+      <c r="B187" s="21" t="s">
+        <v>100</v>
+      </c>
+      <c r="C187" s="21" t="s">
+        <v>125</v>
+      </c>
+      <c r="D187" s="21" t="s">
+        <v>121</v>
+      </c>
+      <c r="E187" s="22">
+        <v>45697.842268518521</v>
+      </c>
+      <c r="F187" s="21">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="188" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A188" s="21" t="s">
+        <v>1324</v>
+      </c>
+      <c r="B188" s="21" t="s">
+        <v>100</v>
+      </c>
+      <c r="C188" s="21" t="s">
+        <v>167</v>
+      </c>
+      <c r="D188" s="21" t="s">
+        <v>121</v>
+      </c>
+      <c r="E188" s="22">
+        <v>45697.845949074072</v>
+      </c>
+      <c r="F188" s="21">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="189" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A189" s="21" t="s">
+        <v>1325</v>
+      </c>
+      <c r="B189" s="21" t="s">
+        <v>100</v>
+      </c>
+      <c r="C189" s="21" t="s">
+        <v>125</v>
+      </c>
+      <c r="D189" s="21" t="s">
+        <v>121</v>
+      </c>
+      <c r="E189" s="22">
+        <v>45697.853055555555</v>
+      </c>
+      <c r="F189" s="21">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="190" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A190" s="21" t="s">
+        <v>1326</v>
+      </c>
+      <c r="B190" s="21" t="s">
+        <v>100</v>
+      </c>
+      <c r="C190" s="21" t="s">
+        <v>167</v>
+      </c>
+      <c r="D190" s="21" t="s">
+        <v>121</v>
+      </c>
+      <c r="E190" s="22">
+        <v>45697.862199074072</v>
+      </c>
+      <c r="F190" s="21">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="191" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A191" s="21" t="s">
+        <v>1327</v>
+      </c>
+      <c r="B191" s="21" t="s">
+        <v>100</v>
+      </c>
+      <c r="C191" s="21" t="s">
+        <v>167</v>
+      </c>
+      <c r="D191" s="21" t="s">
+        <v>121</v>
+      </c>
+      <c r="E191" s="22">
+        <v>45697.866053240738</v>
+      </c>
+      <c r="F191" s="21">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="192" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A192" s="21" t="s">
+        <v>1328</v>
+      </c>
+      <c r="B192" s="21" t="s">
+        <v>100</v>
+      </c>
+      <c r="C192" s="21" t="s">
+        <v>409</v>
+      </c>
+      <c r="D192" s="21" t="s">
+        <v>121</v>
+      </c>
+      <c r="E192" s="22">
+        <v>45697.870474537034</v>
+      </c>
+      <c r="F192" s="21">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="193" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A193" s="21" t="s">
+        <v>1329</v>
+      </c>
+      <c r="B193" s="21" t="s">
+        <v>100</v>
+      </c>
+      <c r="C193" s="21" t="s">
+        <v>259</v>
+      </c>
+      <c r="D193" s="21" t="s">
+        <v>115</v>
+      </c>
+      <c r="E193" s="22">
+        <v>45697.874490740738</v>
+      </c>
+      <c r="F193" s="21">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="194" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A194" s="21" t="s">
+        <v>1330</v>
+      </c>
+      <c r="B194" s="21" t="s">
+        <v>1331</v>
+      </c>
+      <c r="C194" s="21" t="s">
+        <v>169</v>
+      </c>
+      <c r="D194" s="21" t="s">
+        <v>115</v>
+      </c>
+      <c r="E194" s="22">
+        <v>45697.876539351855</v>
+      </c>
+      <c r="F194" s="21">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="195" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A195" s="21" t="s">
+        <v>1332</v>
+      </c>
+      <c r="B195" s="21" t="s">
+        <v>281</v>
+      </c>
+      <c r="C195" s="21" t="s">
+        <v>125</v>
+      </c>
+      <c r="D195" s="21" t="s">
+        <v>121</v>
+      </c>
+      <c r="E195" s="22">
+        <v>45697.879293981481</v>
+      </c>
+      <c r="F195" s="21">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="196" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A196" s="21" t="s">
+        <v>1333</v>
+      </c>
+      <c r="B196" s="21" t="s">
+        <v>133</v>
+      </c>
+      <c r="C196" s="21" t="s">
+        <v>125</v>
+      </c>
+      <c r="D196" s="23" t="s">
+        <v>1334</v>
+      </c>
+      <c r="E196" s="22">
+        <v>45697.88386574074</v>
+      </c>
+      <c r="F196" s="21">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="197" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A197" s="21" t="s">
+        <v>1335</v>
+      </c>
+      <c r="B197" s="21" t="s">
+        <v>91</v>
+      </c>
+      <c r="C197" s="21" t="s">
+        <v>153</v>
+      </c>
+      <c r="D197" s="21" t="s">
+        <v>121</v>
+      </c>
+      <c r="E197" s="21" t="s">
+        <v>1336</v>
+      </c>
+      <c r="F197" s="21">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="198" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A198" s="21" t="s">
+        <v>1337</v>
+      </c>
+      <c r="B198" s="21" t="s">
+        <v>86</v>
+      </c>
+      <c r="C198" s="21" t="s">
+        <v>259</v>
+      </c>
+      <c r="D198" s="21" t="s">
+        <v>115</v>
+      </c>
+      <c r="E198" s="21" t="s">
+        <v>1338</v>
+      </c>
+      <c r="F198" s="21">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="199" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A199" s="21" t="s">
+        <v>1339</v>
+      </c>
+      <c r="B199" s="21" t="s">
+        <v>100</v>
+      </c>
+      <c r="C199" s="21" t="s">
+        <v>167</v>
+      </c>
+      <c r="D199" s="21" t="s">
+        <v>121</v>
+      </c>
+      <c r="E199" s="21" t="s">
+        <v>1340</v>
+      </c>
+      <c r="F199" s="21">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="200" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A200" s="21" t="s">
+        <v>1341</v>
+      </c>
+      <c r="B200" s="21" t="s">
+        <v>100</v>
+      </c>
+      <c r="C200" s="21" t="s">
+        <v>90</v>
+      </c>
+      <c r="D200" s="21" t="s">
+        <v>149</v>
+      </c>
+      <c r="E200" s="21" t="s">
+        <v>1342</v>
+      </c>
+      <c r="F200" s="21">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="201" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A201" s="21" t="s">
+        <v>1343</v>
+      </c>
+      <c r="B201" s="21" t="s">
+        <v>86</v>
+      </c>
+      <c r="C201" s="21" t="s">
+        <v>125</v>
+      </c>
+      <c r="D201" s="21" t="s">
+        <v>121</v>
+      </c>
+      <c r="E201" s="21" t="s">
+        <v>1344</v>
+      </c>
+      <c r="F201" s="21">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="202" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A202" s="21" t="s">
+        <v>1345</v>
+      </c>
+      <c r="B202" s="21" t="s">
+        <v>86</v>
+      </c>
+      <c r="C202" s="21" t="s">
+        <v>167</v>
+      </c>
+      <c r="D202" s="21" t="s">
+        <v>121</v>
+      </c>
+      <c r="E202" s="21" t="s">
+        <v>1346</v>
+      </c>
+      <c r="F202" s="21">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="203" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A203" s="21" t="s">
+        <v>1347</v>
+      </c>
+      <c r="B203" s="21" t="s">
+        <v>86</v>
+      </c>
+      <c r="C203" s="21" t="s">
+        <v>167</v>
+      </c>
+      <c r="D203" s="21" t="s">
+        <v>121</v>
+      </c>
+      <c r="E203" s="21" t="s">
+        <v>1348</v>
+      </c>
+      <c r="F203" s="21">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="204" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A204" s="21" t="s">
+        <v>1349</v>
+      </c>
+      <c r="B204" s="21" t="s">
+        <v>86</v>
+      </c>
+      <c r="C204" s="21" t="s">
+        <v>212</v>
+      </c>
+      <c r="D204" s="21" t="s">
+        <v>121</v>
+      </c>
+      <c r="E204" s="21" t="s">
+        <v>1350</v>
+      </c>
+      <c r="F204" s="21">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="205" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A205" s="21" t="s">
+        <v>1351</v>
+      </c>
+      <c r="B205" s="21" t="s">
+        <v>100</v>
+      </c>
+      <c r="C205" s="21" t="s">
+        <v>409</v>
+      </c>
+      <c r="D205" s="21" t="s">
+        <v>149</v>
+      </c>
+      <c r="E205" s="21" t="s">
+        <v>1352</v>
+      </c>
+      <c r="F205" s="21">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="206" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A206" s="21" t="s">
+        <v>1353</v>
+      </c>
+      <c r="B206" s="21" t="s">
+        <v>91</v>
+      </c>
+      <c r="C206" s="21" t="s">
+        <v>167</v>
+      </c>
+      <c r="D206" s="21" t="s">
+        <v>149</v>
+      </c>
+      <c r="E206" s="21" t="s">
+        <v>1354</v>
+      </c>
+      <c r="F206" s="21">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="207" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A207" s="21" t="s">
+        <v>1355</v>
+      </c>
+      <c r="B207" s="21" t="s">
+        <v>91</v>
+      </c>
+      <c r="C207" s="21" t="s">
+        <v>169</v>
+      </c>
+      <c r="D207" s="21" t="s">
+        <v>149</v>
+      </c>
+      <c r="E207" s="21" t="s">
+        <v>1356</v>
+      </c>
+      <c r="F207" s="21">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="208" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A208" s="21" t="s">
+        <v>1357</v>
+      </c>
+      <c r="B208" s="21" t="s">
+        <v>91</v>
+      </c>
+      <c r="C208" s="21" t="s">
+        <v>125</v>
+      </c>
+      <c r="D208" s="21" t="s">
+        <v>121</v>
+      </c>
+      <c r="E208" s="21" t="s">
+        <v>1358</v>
+      </c>
+      <c r="F208" s="21">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="209" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A209" s="21" t="s">
+        <v>1359</v>
+      </c>
+      <c r="B209" s="21" t="s">
+        <v>91</v>
+      </c>
+      <c r="C209" s="21" t="s">
+        <v>212</v>
+      </c>
+      <c r="D209" s="21" t="s">
+        <v>121</v>
+      </c>
+      <c r="E209" s="21" t="s">
+        <v>1360</v>
+      </c>
+      <c r="F209" s="21">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="210" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A210" s="21" t="s">
+        <v>236</v>
+      </c>
+      <c r="B210" s="21" t="s">
+        <v>100</v>
+      </c>
+      <c r="C210" s="21" t="s">
+        <v>409</v>
+      </c>
+      <c r="D210" s="21" t="s">
+        <v>149</v>
+      </c>
+      <c r="E210" s="21" t="s">
+        <v>1361</v>
+      </c>
+      <c r="F210" s="21">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="211" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A211" s="21" t="s">
+        <v>1362</v>
+      </c>
+      <c r="B211" s="21" t="s">
+        <v>100</v>
+      </c>
+      <c r="C211" s="21" t="s">
+        <v>114</v>
+      </c>
+      <c r="D211" s="21" t="s">
+        <v>121</v>
+      </c>
+      <c r="E211" s="21" t="s">
+        <v>1363</v>
+      </c>
+      <c r="F211" s="21">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="212" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A212" s="21" t="s">
+        <v>1364</v>
+      </c>
+      <c r="B212" s="21" t="s">
+        <v>100</v>
+      </c>
+      <c r="C212" s="21" t="s">
+        <v>259</v>
+      </c>
+      <c r="D212" s="21" t="s">
+        <v>115</v>
+      </c>
+      <c r="E212" s="21" t="s">
+        <v>1365</v>
+      </c>
+      <c r="F212" s="21">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="213" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A213" s="21" t="s">
+        <v>1366</v>
+      </c>
+      <c r="B213" s="21" t="s">
+        <v>100</v>
+      </c>
+      <c r="C213" s="21" t="s">
+        <v>167</v>
+      </c>
+      <c r="D213" s="21" t="s">
+        <v>115</v>
+      </c>
+      <c r="E213" s="21" t="s">
+        <v>1367</v>
+      </c>
+      <c r="F213" s="21">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="214" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A214" s="21" t="s">
+        <v>1368</v>
+      </c>
+      <c r="B214" s="21" t="s">
+        <v>86</v>
+      </c>
+      <c r="C214" s="21" t="s">
+        <v>259</v>
+      </c>
+      <c r="D214" s="21" t="s">
+        <v>115</v>
+      </c>
+      <c r="E214" s="21" t="s">
+        <v>1369</v>
+      </c>
+      <c r="F214" s="21">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="215" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A215" s="21" t="s">
+        <v>1370</v>
+      </c>
+      <c r="B215" s="21" t="s">
+        <v>100</v>
+      </c>
+      <c r="C215" s="21" t="s">
+        <v>212</v>
+      </c>
+      <c r="D215" s="21" t="s">
+        <v>149</v>
+      </c>
+      <c r="E215" s="21" t="s">
+        <v>1371</v>
+      </c>
+      <c r="F215" s="21">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="216" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A216" s="21" t="s">
+        <v>1372</v>
+      </c>
+      <c r="B216" s="21" t="s">
+        <v>100</v>
+      </c>
+      <c r="C216" s="21" t="s">
+        <v>167</v>
+      </c>
+      <c r="D216" s="21" t="s">
+        <v>149</v>
+      </c>
+      <c r="E216" s="21" t="s">
+        <v>1373</v>
+      </c>
+      <c r="F216" s="21">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="217" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A217" s="21" t="s">
+        <v>1374</v>
+      </c>
+      <c r="B217" s="21" t="s">
+        <v>100</v>
+      </c>
+      <c r="C217" s="21" t="s">
+        <v>167</v>
+      </c>
+      <c r="D217" s="21" t="s">
+        <v>115</v>
+      </c>
+      <c r="E217" s="21" t="s">
+        <v>1375</v>
+      </c>
+      <c r="F217" s="21">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="218" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A218" s="21" t="s">
+        <v>1376</v>
+      </c>
+      <c r="B218" s="21" t="s">
+        <v>100</v>
+      </c>
+      <c r="C218" s="21" t="s">
+        <v>259</v>
+      </c>
+      <c r="D218" s="21" t="s">
+        <v>115</v>
+      </c>
+      <c r="E218" s="21" t="s">
+        <v>1377</v>
+      </c>
+      <c r="F218" s="21">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="219" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A219" s="21" t="s">
+        <v>1378</v>
+      </c>
+      <c r="B219" s="21" t="s">
+        <v>100</v>
+      </c>
+      <c r="C219" s="21" t="s">
+        <v>167</v>
+      </c>
+      <c r="D219" s="21" t="s">
+        <v>149</v>
+      </c>
+      <c r="E219" s="21" t="s">
+        <v>1379</v>
+      </c>
+      <c r="F219" s="21">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="220" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A220" s="21" t="s">
+        <v>1380</v>
+      </c>
+      <c r="B220" s="21" t="s">
+        <v>1331</v>
+      </c>
+      <c r="C220" s="21" t="s">
+        <v>114</v>
+      </c>
+      <c r="D220" s="21" t="s">
+        <v>149</v>
+      </c>
+      <c r="E220" s="21" t="s">
+        <v>1381</v>
+      </c>
+      <c r="F220" s="21">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="221" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A221" s="21" t="s">
+        <v>1382</v>
+      </c>
+      <c r="B221" s="21" t="s">
+        <v>91</v>
+      </c>
+      <c r="C221" s="21" t="s">
+        <v>125</v>
+      </c>
+      <c r="D221" s="21" t="s">
+        <v>115</v>
+      </c>
+      <c r="E221" s="21" t="s">
+        <v>1383</v>
+      </c>
+      <c r="F221" s="21">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="222" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A222" s="21" t="s">
+        <v>1384</v>
+      </c>
+      <c r="B222" s="21" t="s">
+        <v>124</v>
+      </c>
+      <c r="C222" s="21" t="s">
+        <v>153</v>
+      </c>
+      <c r="D222" s="21" t="s">
+        <v>115</v>
+      </c>
+      <c r="E222" s="21" t="s">
+        <v>1385</v>
+      </c>
+      <c r="F222" s="21">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="223" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A223" s="21" t="s">
+        <v>1386</v>
+      </c>
+      <c r="B223" s="21" t="s">
+        <v>1331</v>
+      </c>
+      <c r="C223" s="21" t="s">
+        <v>167</v>
+      </c>
+      <c r="D223" s="21" t="s">
+        <v>149</v>
+      </c>
+      <c r="E223" s="21" t="s">
+        <v>1387</v>
+      </c>
+      <c r="F223" s="21">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="224" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A224" s="21" t="s">
+        <v>1388</v>
+      </c>
+      <c r="B224" s="21" t="s">
+        <v>418</v>
+      </c>
+      <c r="C224" s="21" t="s">
+        <v>125</v>
+      </c>
+      <c r="D224" s="21" t="s">
+        <v>115</v>
+      </c>
+      <c r="E224" s="21" t="s">
+        <v>1389</v>
+      </c>
+      <c r="F224" s="21">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="225" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A225" s="21" t="s">
+        <v>1390</v>
+      </c>
+      <c r="B225" s="21" t="s">
+        <v>100</v>
+      </c>
+      <c r="C225" s="21" t="s">
+        <v>374</v>
+      </c>
+      <c r="D225" s="21" t="s">
+        <v>149</v>
+      </c>
+      <c r="E225" s="21" t="s">
+        <v>1391</v>
+      </c>
+      <c r="F225" s="21">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="226" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A226" s="21" t="s">
+        <v>1392</v>
+      </c>
+      <c r="B226" s="21" t="s">
+        <v>100</v>
+      </c>
+      <c r="C226" s="21" t="s">
+        <v>167</v>
+      </c>
+      <c r="D226" s="21" t="s">
+        <v>115</v>
+      </c>
+      <c r="E226" s="21" t="s">
+        <v>1393</v>
+      </c>
+      <c r="F226" s="21">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="227" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A227" s="21" t="s">
+        <v>1394</v>
+      </c>
+      <c r="B227" s="21" t="s">
+        <v>91</v>
+      </c>
+      <c r="C227" s="21" t="s">
+        <v>291</v>
+      </c>
+      <c r="D227" s="21" t="s">
+        <v>115</v>
+      </c>
+      <c r="E227" s="21" t="s">
+        <v>1395</v>
+      </c>
+      <c r="F227" s="21">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="228" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A228" s="21" t="s">
+        <v>1396</v>
+      </c>
+      <c r="B228" s="21" t="s">
+        <v>91</v>
+      </c>
+      <c r="C228" s="21" t="s">
+        <v>167</v>
+      </c>
+      <c r="D228" s="21" t="s">
+        <v>115</v>
+      </c>
+      <c r="E228" s="21" t="s">
+        <v>1397</v>
+      </c>
+      <c r="F228" s="21">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="229" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A229" s="21" t="s">
+        <v>1398</v>
+      </c>
+      <c r="B229" s="21" t="s">
+        <v>91</v>
+      </c>
+      <c r="C229" s="21" t="s">
+        <v>167</v>
+      </c>
+      <c r="D229" s="21" t="s">
+        <v>115</v>
+      </c>
+      <c r="E229" s="21" t="s">
+        <v>1399</v>
+      </c>
+      <c r="F229" s="21">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="230" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A230" s="21" t="s">
+        <v>1400</v>
+      </c>
+      <c r="B230" s="21" t="s">
+        <v>79</v>
+      </c>
+      <c r="C230" s="21" t="s">
+        <v>125</v>
+      </c>
+      <c r="D230" s="21" t="s">
+        <v>121</v>
+      </c>
+      <c r="E230" s="21" t="s">
+        <v>1401</v>
+      </c>
+      <c r="F230" s="21">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="231" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A231" s="21" t="s">
+        <v>286</v>
+      </c>
+      <c r="B231" s="21" t="s">
+        <v>221</v>
+      </c>
+      <c r="C231" s="21" t="s">
+        <v>374</v>
+      </c>
+      <c r="D231" s="21" t="s">
+        <v>149</v>
+      </c>
+      <c r="E231" s="21" t="s">
+        <v>1402</v>
+      </c>
+      <c r="F231" s="21">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="232" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A232" s="21" t="s">
+        <v>1403</v>
+      </c>
+      <c r="B232" s="21" t="s">
+        <v>100</v>
+      </c>
+      <c r="C232" s="21" t="s">
+        <v>167</v>
+      </c>
+      <c r="D232" s="21" t="s">
+        <v>115</v>
+      </c>
+      <c r="E232" s="21" t="s">
+        <v>1404</v>
+      </c>
+      <c r="F232" s="21">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="233" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A233" s="21" t="s">
+        <v>1405</v>
+      </c>
+      <c r="B233" s="21" t="s">
+        <v>100</v>
+      </c>
+      <c r="C233" s="21" t="s">
+        <v>167</v>
+      </c>
+      <c r="D233" s="21" t="s">
+        <v>115</v>
+      </c>
+      <c r="E233" s="21" t="s">
+        <v>1406</v>
+      </c>
+      <c r="F233" s="21">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="234" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A234" s="21" t="s">
+        <v>1407</v>
+      </c>
+      <c r="B234" s="21" t="s">
+        <v>256</v>
+      </c>
+      <c r="C234" s="21" t="s">
+        <v>1408</v>
+      </c>
+      <c r="D234" s="21" t="s">
+        <v>121</v>
+      </c>
+      <c r="E234" s="21" t="s">
+        <v>1409</v>
+      </c>
+      <c r="F234" s="21">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="235" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A235" s="21" t="s">
+        <v>1410</v>
+      </c>
+      <c r="B235" s="21" t="s">
+        <v>86</v>
+      </c>
+      <c r="C235" s="21" t="s">
+        <v>90</v>
+      </c>
+      <c r="D235" s="21" t="s">
+        <v>149</v>
+      </c>
+      <c r="E235" s="21" t="s">
+        <v>1411</v>
+      </c>
+      <c r="F235" s="21">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="236" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A236" s="21" t="s">
+        <v>574</v>
+      </c>
+      <c r="B236" s="21" t="s">
+        <v>86</v>
+      </c>
+      <c r="C236" s="21" t="s">
+        <v>125</v>
+      </c>
+      <c r="D236" s="21" t="s">
+        <v>121</v>
+      </c>
+      <c r="E236" s="21" t="s">
+        <v>1412</v>
+      </c>
+      <c r="F236" s="21">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="237" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A237" s="21" t="s">
+        <v>1413</v>
+      </c>
+      <c r="B237" s="21" t="s">
+        <v>100</v>
+      </c>
+      <c r="C237" s="21" t="s">
+        <v>167</v>
+      </c>
+      <c r="D237" s="21" t="s">
+        <v>115</v>
+      </c>
+      <c r="E237" s="21" t="s">
+        <v>1414</v>
+      </c>
+      <c r="F237" s="21">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="238" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A238" s="21" t="s">
+        <v>1415</v>
+      </c>
+      <c r="B238" s="21" t="s">
+        <v>100</v>
+      </c>
+      <c r="C238" s="21" t="s">
+        <v>125</v>
+      </c>
+      <c r="D238" s="21" t="s">
+        <v>121</v>
+      </c>
+      <c r="E238" s="21" t="s">
+        <v>1416</v>
+      </c>
+      <c r="F238" s="21">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="239" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A239" s="21" t="s">
+        <v>151</v>
+      </c>
+      <c r="B239" s="21" t="s">
+        <v>100</v>
+      </c>
+      <c r="C239" s="21" t="s">
+        <v>114</v>
+      </c>
+      <c r="D239" s="21" t="s">
+        <v>121</v>
+      </c>
+      <c r="E239" s="21" t="s">
+        <v>1417</v>
+      </c>
+      <c r="F239" s="21">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="240" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A240" s="21" t="s">
+        <v>1418</v>
+      </c>
+      <c r="B240" s="21" t="s">
+        <v>86</v>
+      </c>
+      <c r="C240" s="21" t="s">
+        <v>409</v>
+      </c>
+      <c r="D240" s="21" t="s">
+        <v>149</v>
+      </c>
+      <c r="E240" s="21" t="s">
+        <v>1419</v>
+      </c>
+      <c r="F240" s="21">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="241" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A241" s="21" t="s">
+        <v>1420</v>
+      </c>
+      <c r="B241" s="21" t="s">
+        <v>100</v>
+      </c>
+      <c r="C241" s="21" t="s">
+        <v>125</v>
+      </c>
+      <c r="D241" s="21" t="s">
+        <v>121</v>
+      </c>
+      <c r="E241" s="21" t="s">
+        <v>1421</v>
+      </c>
+      <c r="F241" s="21">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="242" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A242" s="21" t="s">
+        <v>1422</v>
+      </c>
+      <c r="B242" s="21" t="s">
+        <v>1331</v>
+      </c>
+      <c r="C242" s="21" t="s">
+        <v>167</v>
+      </c>
+      <c r="D242" s="21" t="s">
+        <v>149</v>
+      </c>
+      <c r="E242" s="21" t="s">
+        <v>1423</v>
+      </c>
+      <c r="F242" s="21">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="243" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A243" s="21" t="s">
+        <v>1424</v>
+      </c>
+      <c r="B243" s="21" t="s">
+        <v>100</v>
+      </c>
+      <c r="C243" s="21" t="s">
+        <v>167</v>
+      </c>
+      <c r="D243" s="21" t="s">
+        <v>149</v>
+      </c>
+      <c r="E243" s="21" t="s">
+        <v>1425</v>
+      </c>
+      <c r="F243" s="21">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="244" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A244" s="21" t="s">
+        <v>1426</v>
+      </c>
+      <c r="B244" s="21" t="s">
+        <v>86</v>
+      </c>
+      <c r="C244" s="21" t="s">
+        <v>374</v>
+      </c>
+      <c r="D244" s="21" t="s">
+        <v>149</v>
+      </c>
+      <c r="E244" s="21" t="s">
+        <v>1427</v>
+      </c>
+      <c r="F244" s="21">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="245" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A245" s="21" t="s">
+        <v>1428</v>
+      </c>
+      <c r="B245" s="21" t="s">
+        <v>100</v>
+      </c>
+      <c r="C245" s="21" t="s">
+        <v>125</v>
+      </c>
+      <c r="D245" s="21" t="s">
+        <v>121</v>
+      </c>
+      <c r="E245" s="21" t="s">
+        <v>1429</v>
+      </c>
+      <c r="F245" s="21">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="246" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A246" s="21" t="s">
+        <v>1430</v>
+      </c>
+      <c r="B246" s="21" t="s">
+        <v>100</v>
+      </c>
+      <c r="C246" s="21" t="s">
+        <v>167</v>
+      </c>
+      <c r="D246" s="21" t="s">
+        <v>115</v>
+      </c>
+      <c r="E246" s="21" t="s">
+        <v>1431</v>
+      </c>
+      <c r="F246" s="21">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="247" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A247" s="21" t="s">
+        <v>533</v>
+      </c>
+      <c r="B247" s="21" t="s">
+        <v>100</v>
+      </c>
+      <c r="C247" s="21" t="s">
+        <v>409</v>
+      </c>
+      <c r="D247" s="21" t="s">
+        <v>115</v>
+      </c>
+      <c r="E247" s="21" t="s">
+        <v>1432</v>
+      </c>
+      <c r="F247" s="21">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="248" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A248" s="21" t="s">
+        <v>1433</v>
+      </c>
+      <c r="B248" s="21" t="s">
+        <v>91</v>
+      </c>
+      <c r="C248" s="21" t="s">
+        <v>125</v>
+      </c>
+      <c r="D248" s="21" t="s">
+        <v>121</v>
+      </c>
+      <c r="E248" s="21" t="s">
+        <v>1434</v>
+      </c>
+      <c r="F248" s="21">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="249" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A249" s="21" t="s">
+        <v>1435</v>
+      </c>
+      <c r="B249" s="21" t="s">
+        <v>86</v>
+      </c>
+      <c r="C249" s="21" t="s">
+        <v>125</v>
+      </c>
+      <c r="D249" s="21" t="s">
+        <v>121</v>
+      </c>
+      <c r="E249" s="21" t="s">
+        <v>1436</v>
+      </c>
+      <c r="F249" s="21">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="250" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A250" s="21" t="s">
+        <v>1437</v>
+      </c>
+      <c r="B250" s="21" t="s">
+        <v>91</v>
+      </c>
+      <c r="C250" s="21" t="s">
+        <v>125</v>
+      </c>
+      <c r="D250" s="21" t="s">
+        <v>121</v>
+      </c>
+      <c r="E250" s="21" t="s">
+        <v>1438</v>
+      </c>
+      <c r="F250" s="21">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="251" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A251" s="21" t="s">
+        <v>1439</v>
+      </c>
+      <c r="B251" s="21" t="s">
+        <v>323</v>
+      </c>
+      <c r="C251" s="21" t="s">
+        <v>167</v>
+      </c>
+      <c r="D251" s="21" t="s">
+        <v>115</v>
+      </c>
+      <c r="E251" s="21" t="s">
+        <v>1440</v>
+      </c>
+      <c r="F251" s="21">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="252" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A252" s="21" t="s">
+        <v>511</v>
+      </c>
+      <c r="B252" s="21" t="s">
+        <v>100</v>
+      </c>
+      <c r="C252" s="21" t="s">
+        <v>125</v>
+      </c>
+      <c r="D252" s="21" t="s">
+        <v>121</v>
+      </c>
+      <c r="E252" s="21" t="s">
+        <v>1441</v>
+      </c>
+      <c r="F252" s="21">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="253" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A253" s="21" t="s">
+        <v>1442</v>
+      </c>
+      <c r="B253" s="21" t="s">
+        <v>86</v>
+      </c>
+      <c r="C253" s="21" t="s">
+        <v>167</v>
+      </c>
+      <c r="D253" s="21" t="s">
+        <v>121</v>
+      </c>
+      <c r="E253" s="21" t="s">
+        <v>1443</v>
+      </c>
+      <c r="F253" s="21">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="254" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A254" s="21" t="s">
+        <v>1444</v>
+      </c>
+      <c r="B254" s="21" t="s">
+        <v>100</v>
+      </c>
+      <c r="C254" s="21" t="s">
+        <v>125</v>
+      </c>
+      <c r="D254" s="21" t="s">
+        <v>121</v>
+      </c>
+      <c r="E254" s="21" t="s">
+        <v>1445</v>
+      </c>
+      <c r="F254" s="21">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="255" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A255" s="21" t="s">
+        <v>1446</v>
+      </c>
+      <c r="B255" s="21" t="s">
+        <v>100</v>
+      </c>
+      <c r="C255" s="21" t="s">
+        <v>409</v>
+      </c>
+      <c r="D255" s="21" t="s">
+        <v>121</v>
+      </c>
+      <c r="E255" s="21" t="s">
+        <v>1447</v>
+      </c>
+      <c r="F255" s="21">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="256" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A256" s="21" t="s">
+        <v>1448</v>
+      </c>
+      <c r="B256" s="21" t="s">
+        <v>100</v>
+      </c>
+      <c r="C256" s="21" t="s">
+        <v>125</v>
+      </c>
+      <c r="D256" s="21" t="s">
+        <v>121</v>
+      </c>
+      <c r="E256" s="21" t="s">
+        <v>1449</v>
+      </c>
+      <c r="F256" s="21">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="257" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A257" s="21" t="s">
+        <v>1450</v>
+      </c>
+      <c r="B257" s="21" t="s">
+        <v>100</v>
+      </c>
+      <c r="C257" s="21" t="s">
+        <v>409</v>
+      </c>
+      <c r="D257" s="21" t="s">
+        <v>121</v>
+      </c>
+      <c r="E257" s="21" t="s">
+        <v>1451</v>
+      </c>
+      <c r="F257" s="21">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="258" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A258" s="21" t="s">
+        <v>1452</v>
+      </c>
+      <c r="B258" s="21" t="s">
+        <v>100</v>
+      </c>
+      <c r="C258" s="21" t="s">
+        <v>409</v>
+      </c>
+      <c r="D258" s="21" t="s">
+        <v>121</v>
+      </c>
+      <c r="E258" s="21" t="s">
+        <v>1453</v>
+      </c>
+      <c r="F258" s="21">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="259" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A259" s="21" t="s">
+        <v>1454</v>
+      </c>
+      <c r="B259" s="21" t="s">
+        <v>100</v>
+      </c>
+      <c r="C259" s="21" t="s">
+        <v>167</v>
+      </c>
+      <c r="D259" s="21" t="s">
+        <v>115</v>
+      </c>
+      <c r="E259" s="21" t="s">
+        <v>1455</v>
+      </c>
+      <c r="F259" s="21">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="260" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A260" s="21" t="s">
+        <v>1456</v>
+      </c>
+      <c r="B260" s="21" t="s">
+        <v>342</v>
+      </c>
+      <c r="C260" s="21" t="s">
+        <v>125</v>
+      </c>
+      <c r="D260" s="21" t="s">
+        <v>121</v>
+      </c>
+      <c r="E260" s="21" t="s">
+        <v>1457</v>
+      </c>
+      <c r="F260" s="21">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="261" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A261" s="21" t="s">
+        <v>359</v>
+      </c>
+      <c r="B261" s="21" t="s">
+        <v>91</v>
+      </c>
+      <c r="C261" s="21" t="s">
+        <v>167</v>
+      </c>
+      <c r="D261" s="21" t="s">
+        <v>115</v>
+      </c>
+      <c r="E261" s="21" t="s">
+        <v>1458</v>
+      </c>
+      <c r="F261" s="21">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="262" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A262" s="21" t="s">
+        <v>549</v>
+      </c>
+      <c r="B262" s="21" t="s">
+        <v>100</v>
+      </c>
+      <c r="C262" s="21" t="s">
+        <v>409</v>
+      </c>
+      <c r="D262" s="21" t="s">
+        <v>121</v>
+      </c>
+      <c r="E262" s="21" t="s">
+        <v>1459</v>
+      </c>
+      <c r="F262" s="21">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="263" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A263" s="21" t="s">
+        <v>1460</v>
+      </c>
+      <c r="B263" s="21" t="s">
+        <v>1461</v>
+      </c>
+      <c r="C263" s="21" t="s">
+        <v>167</v>
+      </c>
+      <c r="D263" s="21" t="s">
+        <v>121</v>
+      </c>
+      <c r="E263" s="21" t="s">
+        <v>1462</v>
+      </c>
+      <c r="F263" s="21">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="264" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A264" s="21" t="s">
+        <v>1463</v>
+      </c>
+      <c r="B264" s="21" t="s">
+        <v>124</v>
+      </c>
+      <c r="C264" s="21" t="s">
+        <v>167</v>
+      </c>
+      <c r="D264" s="21" t="s">
+        <v>115</v>
+      </c>
+      <c r="E264" s="21" t="s">
+        <v>1464</v>
+      </c>
+      <c r="F264" s="21">
+        <v>8</v>
+      </c>
+    </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="custom" allowBlank="1" showDropDown="1" sqref="E2:E157" xr:uid="{00000000-0002-0000-0100-000000000000}">
+    <dataValidation type="custom" allowBlank="1" showDropDown="1" sqref="E2:E264" xr:uid="{00000000-0002-0000-0100-000000000000}">
       <formula1>OR(NOT(ISERROR(DATEVALUE(E2))), AND(ISNUMBER(E2), LEFT(CELL("format", E2))="D"))</formula1>
     </dataValidation>
   </dataValidations>
+  <hyperlinks>
+    <hyperlink ref="D196" r:id="rId1" xr:uid="{E2C00380-639D-CF45-9639-3D4759DEA411}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>

</xml_diff>